<commit_message>
all experiments are run with initial network as reference point
</commit_message>
<xml_diff>
--- a/results/AVEA/results.xlsx
+++ b/results/AVEA/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-riaktu\IdeaProjects\graph2vec\results\AVEA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96D05DC5-A159-432B-8C92-C1E07E4FDE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842134B6-8012-4ACD-B5C9-EC9B0E956A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dists" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>2, 3, 4, 5, 6, 11, 16, 17, 18, 22, 24, 25, 29, 30</t>
+  </si>
+  <si>
+    <t>euclidian</t>
+  </si>
+  <si>
+    <t>cosine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -506,7 +512,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
@@ -633,96 +640,99 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>dists!$B$2:$B$30</c:f>
+              <c:f>dists!$B$2:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0.67500573848767897</c:v>
+                  <c:v>2.7619448972621301</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6126477057331901</c:v>
+                  <c:v>2.9390338495563202</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.87832921419563903</c:v>
+                  <c:v>1.58016384875587</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0743240342921001</c:v>
+                  <c:v>1.92720252138628</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.96360658604041505</c:v>
+                  <c:v>1.5808192007328601</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.53435970562541402</c:v>
+                  <c:v>1.9115383073174099</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.65088144071324805</c:v>
+                  <c:v>2.1522524940226702</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.96830064981604103</c:v>
+                  <c:v>2.48280724004595</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4947426841195299</c:v>
+                  <c:v>3.0558334475984199</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.62470781163997602</c:v>
+                  <c:v>1.92313775311917</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.66385076834412204</c:v>
+                  <c:v>1.79451113293817</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.647975657042272</c:v>
+                  <c:v>1.7835167382966199</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.77247630839604098</c:v>
+                  <c:v>1.96340507551015</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.33015878200372</c:v>
+                  <c:v>2.1522496698909599</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.3745425985686199</c:v>
+                  <c:v>2.3619387231851001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.56680819797517</c:v>
+                  <c:v>2.8422347676881801</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.90428800820389998</c:v>
+                  <c:v>1.64248900987415</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.1007797033009901</c:v>
+                  <c:v>2.0861433732631798</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.57147554310495996</c:v>
+                  <c:v>1.6938966537147699</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.662722186941889</c:v>
+                  <c:v>1.83232711457886</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.97804828900555396</c:v>
+                  <c:v>1.94185527153154</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.92133177828880597</c:v>
+                  <c:v>2.4994440810039902</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.80207065247455</c:v>
+                  <c:v>3.0417989852332101</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.1357487592064299</c:v>
+                  <c:v>1.94391790276167</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.39341133079093299</c:v>
+                  <c:v>2.1737111249053598</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.13924593817357</c:v>
+                  <c:v>1.97864578403203</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.07762610213881</c:v>
+                  <c:v>2.2212519824536798</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.08735763917748</c:v>
+                  <c:v>1.6628412373502199</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.56740365287563299</c:v>
+                  <c:v>1.94499568001289</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.4752928839353801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -731,6 +741,341 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5A89-4AA1-A262-9BDB0C5A66E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1447077807"/>
+        <c:axId val="1447061167"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1447077807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1447061167"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1447061167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1447077807"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>dists!$C$2:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1.23196680210445E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3266045084293999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3899669292379803E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3759793438526897E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1675585206430998E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.9676606011131996E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6065961192182101E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9686474970214194E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.49342734658349E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.2134894670247097E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.5137183142759299E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.7661902041284902E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.6763062646444304E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.6431193951677001E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.1493838306986302E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.26455862354943E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.5081865297137398E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.4857407219971403E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.9576682912788597E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.7559748355507897E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.1107085810877503E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.04176232132681E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.5040978509316001E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.4127126695219198E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.4764882648130594E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.8529040695903803E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.4720347976751107E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.7437513911859899E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.6188594534045599E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.1457509577322895E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FD61-4DC5-BAB8-5A0328C25222}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -938,7 +1283,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1487,6 +2388,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>434975</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE3B61DF-C463-4AD6-BB62-33D9CA603305}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1791,253 +2730,355 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="B1">
-        <v>0</v>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0.67500573848767897</v>
+      <c r="B2" s="1">
+        <v>2.7619448972621301</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.23196680210445E-2</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>1.6126477057331901</v>
+      <c r="B3" s="1">
+        <v>2.9390338495563202</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.3266045084293999E-2</v>
       </c>
       <c r="AA3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0.87832921419563903</v>
+      <c r="B4" s="1">
+        <v>1.58016384875587</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.3899669292379803E-3</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>1.0743240342921001</v>
+      <c r="B5" s="1">
+        <v>1.92720252138628</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5.3759793438526897E-3</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>0.96360658604041505</v>
+      <c r="B6" s="1">
+        <v>1.5808192007328601</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.1675585206430998E-3</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>0.53435970562541402</v>
+      <c r="B7" s="1">
+        <v>1.9115383073174099</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5.9676606011131996E-3</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>0.65088144071324805</v>
+      <c r="B8" s="1">
+        <v>2.1522524940226702</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7.6065961192182101E-3</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>0.96830064981604103</v>
+      <c r="B9" s="1">
+        <v>2.48280724004595</v>
+      </c>
+      <c r="C9" s="1">
+        <v>9.9686474970214194E-3</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>1.4947426841195299</v>
+      <c r="B10" s="1">
+        <v>3.0558334475984199</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.49342734658349E-2</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>0.62470781163997602</v>
+      <c r="B11" s="1">
+        <v>1.92313775311917</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6.2134894670247097E-3</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>0.66385076834412204</v>
+      <c r="B12" s="1">
+        <v>1.79451113293817</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5.5137183142759299E-3</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>0.647975657042272</v>
+      <c r="B13" s="1">
+        <v>1.7835167382966199</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5.7661902041284902E-3</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>0.77247630839604098</v>
+      <c r="B14" s="1">
+        <v>1.96340507551015</v>
+      </c>
+      <c r="C14" s="1">
+        <v>6.6763062646444304E-3</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>1.33015878200372</v>
+      <c r="B15" s="1">
+        <v>2.1522496698909599</v>
+      </c>
+      <c r="C15" s="1">
+        <v>8.6431193951677001E-3</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>1.3745425985686199</v>
+      <c r="B16" s="1">
+        <v>2.3619387231851001</v>
+      </c>
+      <c r="C16" s="1">
+        <v>9.1493838306986302E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>1.56680819797517</v>
+      <c r="B17" s="1">
+        <v>2.8422347676881801</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.26455862354943E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>0.90428800820389998</v>
+      <c r="B18" s="1">
+        <v>1.64248900987415</v>
+      </c>
+      <c r="C18" s="1">
+        <v>4.5081865297137398E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>1.1007797033009901</v>
+      <c r="B19" s="1">
+        <v>2.0861433732631798</v>
+      </c>
+      <c r="C19" s="1">
+        <v>7.4857407219971403E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>0.57147554310495996</v>
+      <c r="B20" s="1">
+        <v>1.6938966537147699</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4.9576682912788597E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>0.662722186941889</v>
+      <c r="B21" s="1">
+        <v>1.83232711457886</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5.7559748355507897E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>0.97804828900555396</v>
+      <c r="B22" s="1">
+        <v>1.94185527153154</v>
+      </c>
+      <c r="C22" s="1">
+        <v>6.1107085810877503E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>0.92133177828880597</v>
+      <c r="B23" s="1">
+        <v>2.4994440810039902</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1.04176232132681E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>1.80207065247455</v>
+      <c r="B24" s="1">
+        <v>3.0417989852332101</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1.5040978509316001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25">
-        <v>1.1357487592064299</v>
+      <c r="B25" s="1">
+        <v>1.94391790276167</v>
+      </c>
+      <c r="C25" s="1">
+        <v>6.4127126695219198E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>0.39341133079093299</v>
+      <c r="B26" s="1">
+        <v>2.1737111249053598</v>
+      </c>
+      <c r="C26" s="1">
+        <v>8.4764882648130594E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27">
-        <v>1.13924593817357</v>
+      <c r="B27" s="1">
+        <v>1.97864578403203</v>
+      </c>
+      <c r="C27" s="1">
+        <v>6.8529040695903803E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28">
-        <v>1.07762610213881</v>
+      <c r="B28" s="1">
+        <v>2.2212519824536798</v>
+      </c>
+      <c r="C28" s="1">
+        <v>9.4720347976751107E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29">
-        <v>1.08735763917748</v>
+      <c r="B29" s="1">
+        <v>1.6628412373502199</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4.7437513911859899E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30">
-        <v>0.56740365287563299</v>
+      <c r="B30" s="1">
+        <v>1.94499568001289</v>
+      </c>
+      <c r="C30" s="1">
+        <v>4.6188594534045599E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2.4752928839353801</v>
+      </c>
+      <c r="C31" s="1">
+        <v>8.1457509577322895E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>